<commit_message>
add bom for drumbox
</commit_message>
<xml_diff>
--- a/HiHat + Snare/bom/HiHat+Snare_BOM.xlsx
+++ b/HiHat + Snare/bom/HiHat+Snare_BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asaun\Documents\Perso\Synth\HiHat + Snare\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Documents\synthe modulaire\Synth\HiHat + Snare\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88742B9-498B-4AAD-BC06-8DE9CF904C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02F009F-16A2-4C1F-9D90-D9FEABF3D451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -966,20 +968,20 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="50.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>47</v>
       </c>
@@ -1032,7 +1034,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
@@ -1059,7 +1061,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
         <v>48</v>
       </c>
@@ -1086,7 +1088,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -1113,7 +1115,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1140,7 +1142,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -1167,7 +1169,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>51</v>
       </c>
@@ -1194,7 +1196,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1219,7 +1221,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>57</v>
       </c>
@@ -1246,7 +1248,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>58</v>
       </c>
@@ -1273,7 +1275,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>60</v>
       </c>
@@ -1300,7 +1302,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>61</v>
       </c>
@@ -1327,7 +1329,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>63</v>
       </c>
@@ -1354,7 +1356,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>64</v>
       </c>
@@ -1384,7 +1386,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>66</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>67</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
         <v>96</v>
       </c>
@@ -1463,7 +1465,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
         <v>68</v>
       </c>
@@ -1490,7 +1492,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>72</v>
       </c>
@@ -1515,7 +1517,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
         <v>71</v>
       </c>
@@ -1540,7 +1542,7 @@
         <v>3.3879999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1565,7 +1567,7 @@
         <v>1.694</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
         <v>69</v>
       </c>
@@ -1590,7 +1592,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="27" t="s">
         <v>73</v>
       </c>
@@ -1615,7 +1617,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -1641,7 +1643,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -1667,7 +1669,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>85</v>
       </c>
@@ -1693,7 +1695,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
@@ -1719,7 +1721,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
@@ -1745,7 +1747,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="20" t="s">
         <v>91</v>
       </c>
@@ -1771,7 +1773,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G31" s="13" t="s">
         <v>7</v>
       </c>

</xml_diff>